<commit_message>
10 es poco jajaja
</commit_message>
<xml_diff>
--- a/docs/Datos RedBlack.xlsx
+++ b/docs/Datos RedBlack.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbelt\Downloads\Talleres\T6_202010\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Desktop\Bobi\Estructuras de Datos\Talleres\T6_202010\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B9C056-84AE-482F-8944-328754678EB0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4E6003-5CDA-4A2D-B27B-A4925E6815D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{C83540D4-8C99-4B8D-8D8B-84BD1ED944F4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C83540D4-8C99-4B8D-8D8B-84BD1ED944F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -580,17 +580,17 @@
   <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="71.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="71.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -599,7 +599,7 @@
       </c>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -608,14 +608,16 @@
       </c>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -627,7 +629,7 @@
         <v>19.009186210074169</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -638,7 +640,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>4</v>
       </c>
@@ -650,7 +652,7 @@
         <v>11.99346117111604</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="7" t="s">
         <v>5</v>
       </c>
@@ -662,7 +664,7 @@
         <v>19.009186210074169</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>6</v>
       </c>

</xml_diff>